<commit_message>
&&& - 81814034 от 25.09.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Cyprus/#EURO#Cyprus#Commemorative#[2009-present]#UNC.xlsx
+++ b/Collections/EURO/Cyprus/#EURO#Cyprus#Commemorative#[2009-present]#UNC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Cyprus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17876CF8-2A6F-4A32-9C0C-9543235AD327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5B0037-14C3-4D85-ABB3-40B9BFAB5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3830" yWindow="1090" windowWidth="33150" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -252,7 +255,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -317,8 +320,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +362,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6C3A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +480,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -526,6 +542,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -553,8 +572,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -562,15 +581,7 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BE5FF"/>
-          <bgColor rgb="FF9BE5FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -793,9 +804,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="2" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1070,7 +1081,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1086,27 +1097,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="30"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="24" t="s">
         <v>34</v>
       </c>
@@ -1619,7 +1630,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="10" t="str">
-        <f t="shared" ref="J17:J18" si="4">IF(OR(AND(H17&gt;1,H17&lt;&gt;"-"),AND(I17&gt;1,I17&lt;&gt;"-")),"Can exchange","")</f>
+        <f t="shared" ref="J17" si="4">IF(OR(AND(H17&gt;1,H17&lt;&gt;"-"),AND(I17&gt;1,I17&lt;&gt;"-")),"Can exchange","")</f>
         <v/>
       </c>
     </row>
@@ -1637,14 +1648,14 @@
       <c r="E18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="25" t="s">
         <v>43</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="9">
-        <v>0</v>
+      <c r="H18" s="35">
+        <v>1</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>4</v>
@@ -1671,11 +1682,28 @@
     <mergeCell ref="C1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:I6 H3:H5 H11:I11">
-    <cfRule type="containsText" dxfId="27" priority="61" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="26" priority="63" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:I6 H3:H5 H11:I11">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="containsText" dxfId="25" priority="61" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1687,12 +1715,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="26" priority="59" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+  <conditionalFormatting sqref="I4:I5">
+    <cfRule type="containsText" dxfId="24" priority="59" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I5">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1704,12 +1732,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I5">
-    <cfRule type="containsText" dxfId="25" priority="57" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I5">
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="23" priority="57" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1721,12 +1749,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="24" priority="55" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H7))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="I7">
+    <cfRule type="containsText" dxfId="22" priority="55" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1738,12 +1766,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="containsText" dxfId="23" priority="53" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I7))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="21" priority="53" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1755,12 +1783,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="22" priority="51" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="I8">
+    <cfRule type="containsText" dxfId="20" priority="51" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1772,29 +1800,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="containsText" dxfId="21" priority="49" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H9:I9">
-    <cfRule type="containsText" dxfId="20" priority="43" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="19" priority="45" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:I9">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="18" priority="43" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1806,12 +1834,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="19" priority="41" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="I10">
+    <cfRule type="containsText" dxfId="17" priority="41" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1823,12 +1851,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="containsText" dxfId="18" priority="39" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
+  <conditionalFormatting sqref="H12">
+    <cfRule type="containsText" dxfId="16" priority="39" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1840,12 +1868,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="17" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+  <conditionalFormatting sqref="I12">
+    <cfRule type="containsText" dxfId="15" priority="37" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1857,12 +1885,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="containsText" dxfId="16" priority="35" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="14" priority="35" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1874,12 +1902,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="15" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="I13">
+    <cfRule type="containsText" dxfId="13" priority="33" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1891,29 +1919,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="14" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H14:I14">
-    <cfRule type="containsText" dxfId="13" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="12" priority="27" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:I14">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="11" priority="25" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1925,12 +1953,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="I15">
+    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1942,12 +1970,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
+  <conditionalFormatting sqref="I16">
+    <cfRule type="containsText" dxfId="9" priority="21" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1959,30 +1987,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="10" priority="19" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="8" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1994,11 +2005,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2010,30 +2038,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>

</xml_diff>